<commit_message>
show sample excel, download slip pdf implemented
styling and refactoring code
</commit_message>
<xml_diff>
--- a/emails-bingo-users.xlsx
+++ b/emails-bingo-users.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding_Workspace\BingoMultiplayerGame\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDBA8E89-C1D7-42A1-B2A9-1EEA3EA3F221}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF47029-D329-4B68-9F79-D0366DDC6277}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,12 +26,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Emails</t>
   </si>
   <si>
     <t>somemail@random.com</t>
+  </si>
+  <si>
+    <t>abc@example.com</t>
+  </si>
+  <si>
+    <t>anyone@some.com</t>
   </si>
 </sst>
 </file>
@@ -363,7 +369,7 @@
   <dimension ref="A1:XFD14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -379,7 +385,9 @@
       </c>
     </row>
     <row r="3" spans="1:16384" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -16765,7 +16773,9 @@
       <c r="XFD3" s="1"/>
     </row>
     <row r="4" spans="1:16384" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:16384" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
@@ -16779,9 +16789,11 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{B3EFC9B6-B1E6-4F69-8A1A-42056B612696}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{9D8B2EBA-ED9D-466A-8CD9-3B5AA17DF76E}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{BEA7FF73-8FCE-4C6F-8343-A4B2D2B7BFF7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>